<commit_message>
removes 3rd column from procedures workbook, fixes 15x > issue, sets cc summary review table width to 700px
</commit_message>
<xml_diff>
--- a/templates/procedures.xlsx
+++ b/templates/procedures.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>All Procedures for Study X</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Associated CPT Code</t>
-  </si>
-  <si>
-    <t>Cost to Run at Your Site</t>
   </si>
 </sst>
 </file>
@@ -122,7 +119,9 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -131,18 +130,22 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,15 +497,14 @@
     <col min="4" max="4" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -512,213 +514,185 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
updates module to expect 100 procedure fields, not 25 -- updates workbook template to have 100 proc rows
</commit_message>
<xml_diff>
--- a/templates/procedures.xlsx
+++ b/templates/procedures.xlsx
@@ -33,18 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>All Procedures for Study X</t>
   </si>
   <si>
-    <t>Procedure Name</t>
-  </si>
-  <si>
     <t>Procedure Number</t>
-  </si>
-  <si>
-    <t>Associated CPT Code</t>
   </si>
 </sst>
 </file>
@@ -483,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,14 +500,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -689,6 +679,531 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Fix proc download, gng accepting, and others
</commit_message>
<xml_diff>
--- a/templates/procedures.xlsx
+++ b/templates/procedures.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\redcap\modules\tin_budget_v1.0.0\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app001\www\redcap\modules\TIN-Budget_v1.0\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD2B269-9048-4A5C-B72A-3ADAFC551D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19020" windowHeight="14235"/>
+    <workbookView xWindow="46410" yWindow="7230" windowWidth="20715" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,18 +34,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>All Procedures for Study X</t>
   </si>
   <si>
     <t>Procedure Number</t>
   </si>
+  <si>
+    <t>Procedure Name</t>
+  </si>
+  <si>
+    <t>Associated CPT Code</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,11 +483,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,8 +509,12 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">

</xml_diff>